<commit_message>
updated scrum and such
</commit_message>
<xml_diff>
--- a/scrum/burndown_template.xlsx
+++ b/scrum/burndown_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msudenver-my.sharepoint.com/personal/tmota_msudenver_edu/Documents/Teaching/Courses/__24SCS3250_SE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{7397B228-E7AA-634C-96A5-F3624B942EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AD2388D-B87A-4E1C-9B2A-667F46492534}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{7397B228-E7AA-634C-96A5-F3624B942EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9940FA87-491D-45DF-9226-ACCD54CD1A0D}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15020" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
   </bookViews>
@@ -294,7 +294,7 @@
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,7 +351,7 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -445,7 +445,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>35</c:v>
@@ -1601,7 +1601,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="3">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1616,7 +1616,7 @@
         <v>55</v>
       </c>
       <c r="E3" s="4">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1639,11 +1639,11 @@
         <v>7</v>
       </c>
       <c r="B5" s="4">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4">
         <f>B5-C3</f>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D5" s="4">
         <v>35</v>

</xml_diff>